<commit_message>
Refresh punto 1 tp2
</commit_message>
<xml_diff>
--- a/TP2/Ejercicio 1(Germo)/Mediciones.xlsx
+++ b/TP2/Ejercicio 1(Germo)/Mediciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guido\Documents\GitHub\LABO\TP2\Ejercicio 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\germa\Documents\GitHub\LABO\TP2\Ejercicio 1(Germo)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8B2A90-0E1E-4FDA-B421-CABD0C20DB6D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48999642-C290-4B18-93BA-EECD92E6F924}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D4D8D5A0-A79E-477C-9145-654BD95F2316}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D4D8D5A0-A79E-477C-9145-654BD95F2316}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>